<commit_message>
updated function add and method for the same
</commit_message>
<xml_diff>
--- a/schedule/NewSchedule(Date).xlsx
+++ b/schedule/NewSchedule(Date).xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Date3" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Date1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1 bj3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ddddddd</t>
+          <t>dfgbd</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>dfb</t>
+          <t>fbv</t>
         </is>
       </c>
     </row>
@@ -481,17 +481,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2 bj3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>fb</t>
+          <t>dfbv</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>dfb</t>
+          <t>dfcv</t>
         </is>
       </c>
     </row>
@@ -501,17 +501,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3 bje</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>xfb</t>
+          <t>sdzdgvc</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>xxfb</t>
+          <t>svc</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated serial no and fixes bugs till del
</commit_message>
<xml_diff>
--- a/schedule/NewSchedule(Date).xlsx
+++ b/schedule/NewSchedule(Date).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1 bj3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dfgbd</t>
+          <t>dfg</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>fbv</t>
+          <t>dfg</t>
         </is>
       </c>
     </row>
@@ -481,17 +481,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2 bj3</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dfbv</t>
+          <t>fdg</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>dfcv</t>
+          <t>dfg</t>
         </is>
       </c>
     </row>
@@ -501,17 +501,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3 bje</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>sdzdgvc</t>
+          <t>dfg</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>svc</t>
+          <t>dfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>dfg</t>
         </is>
       </c>
     </row>

</xml_diff>